<commit_message>
Incorporate edits from WRI
</commit_message>
<xml_diff>
--- a/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
+++ b/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr hidePivotFieldList="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EvelineDB\Dropbox\Projeto EPS-WRI\elec_Eveline\Apil 2020\variables corrected\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\elec\BECF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7303FAD5-E7C8-48AE-BE99-64202C218075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabel 1 - Pereira et al" sheetId="9" r:id="rId2"/>
+    <sheet name="Capacity factors" sheetId="9" r:id="rId2"/>
     <sheet name="BECF-pre-ret" sheetId="4" r:id="rId3"/>
     <sheet name="BECF-pre-nonret" sheetId="5" r:id="rId4"/>
     <sheet name="BECF-new" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Source:</t>
   </si>
@@ -115,16 +116,10 @@
     <t>Title</t>
   </si>
   <si>
-    <t>The base data is taken by Pereira et al 2016.</t>
-  </si>
-  <si>
     <t xml:space="preserve">It assumed the mean value of the technologies that shown a range of capacity factor. </t>
   </si>
   <si>
     <t xml:space="preserve">It is assumed the technology of biomass with co-generation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Table 1 - Pereira et al" has the description system of each tecnology </t>
   </si>
   <si>
     <t>Existing Capacity Factors, Except for Coal (and capacity factor for newly built Nuclear)</t>
@@ -163,26 +158,50 @@
     <t>Assumtions:</t>
   </si>
   <si>
-    <t>For BECF-new is considered values of the year 2050 by Pereira et al 2016.</t>
-  </si>
-  <si>
-    <t>For BECF-ret is considered values of the year 2010 by Pereira et al 2016.</t>
-  </si>
-  <si>
     <t>Lignite is assumed to be coal</t>
   </si>
   <si>
     <t>This variable represents the capacity factors that electricity suppliers expect to run each type of power plant in Brazil. Given the choice, an electricity supplier would sooner build a new nonpeaker power plant than attempt to rely on running a nonpeaker plant at greater than its Expected Capacity Factor.</t>
   </si>
+  <si>
+    <t>Newly Built Target Electricity Capacity Factors (OCGT, CCGT)</t>
+  </si>
+  <si>
+    <t>Maurício Tolmasquim (org.)</t>
+  </si>
+  <si>
+    <t>Energia Termelétrica: Gás natural, Biomassa, Carvão, Nuclear</t>
+  </si>
+  <si>
+    <t>https://www.epe.gov.br/sites-pt/publicacoes-dados-abertos/publicacoes/PublicacoesArquivos/publicacao-173/Energia%20Termel%C3%A9trica%20-%20Online%2013maio2016.pdf</t>
+  </si>
+  <si>
+    <t>Table 10</t>
+  </si>
+  <si>
+    <t>The base data is taken by Pereira et al 2016 and Tolmasquim 2016.</t>
+  </si>
+  <si>
+    <t>For BECF-ret is considered values of the year 2010 by Pereira et al 2016 (except OCGT plants).</t>
+  </si>
+  <si>
+    <t>For BECF-new is considered values of the year 2050 by Pereira et al 2016 (except OCGT plants).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Table 1 - Pereira et al" and "Table 10 - Tolmasquim" has the description system of each tecnology </t>
+  </si>
+  <si>
+    <t>For BECF-new and BECF-ret OCGT plants is considered values of the Tolmasquim 2016.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +233,14 @@
       <color rgb="FF0F80AC"/>
       <name val="AdvOT863180fb"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -238,11 +265,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -278,13 +306,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -337,6 +367,50 @@
         <a:xfrm>
           <a:off x="2849879" y="0"/>
           <a:ext cx="7853141" cy="5912458"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>395572</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB4E129-E0E3-2F4A-B43A-C1924D67FDE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3581400" y="6502400"/>
+          <a:ext cx="7799672" cy="1981200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -610,14 +684,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="99.33203125" customWidth="1"/>
@@ -633,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="9"/>
     </row>
@@ -687,7 +761,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="B12" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9"/>
     </row>
@@ -723,7 +797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="2:3">
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
@@ -731,7 +805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="2:3">
       <c r="B18" s="9" t="s">
         <v>21</v>
       </c>
@@ -739,13 +813,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="2:3">
       <c r="B21" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="2:3">
       <c r="B22" s="9" t="s">
         <v>23</v>
       </c>
@@ -753,7 +827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="2:3">
       <c r="B23" s="9" t="s">
         <v>25</v>
       </c>
@@ -761,7 +835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="2:3">
       <c r="B24" s="9" t="s">
         <v>16</v>
       </c>
@@ -769,7 +843,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="2:3">
       <c r="B25" s="9" t="s">
         <v>17</v>
       </c>
@@ -777,7 +851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="2:3">
       <c r="B26" s="9" t="s">
         <v>19</v>
       </c>
@@ -785,7 +859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="2:3">
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -793,103 +867,161 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+    <row r="29" spans="2:3">
+      <c r="B29" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="B33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35" s="14"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="48.6" customHeight="1">
-      <c r="A31" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="12"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="12" t="s">
+    <row r="37" spans="1:3" ht="48.5" customHeight="1">
+      <c r="A37" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="12"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="12"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="18" customFormat="1">
+      <c r="A46" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="12"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" s="18" customFormat="1">
-      <c r="A39" s="17" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="12" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="12" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C33" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7DF09F-4E3B-40EB-8176-26BC6F884491}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="43.2">
+    <row r="2" spans="1:3" ht="42.75">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -902,7 +1034,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -913,7 +1045,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4">
         <v>0.55000000000000004</v>
@@ -979,7 +1111,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6">
         <v>0.245</v>
@@ -1015,10 +1147,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="4">
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="C13" s="4">
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1045,7 +1177,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6">
         <v>0.2</v>
@@ -1056,7 +1188,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6">
         <v>0.54</v>
@@ -1083,23 +1215,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="4" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.46484375" customWidth="1"/>
+    <col min="2" max="4" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="28.8">
+    <row r="1" spans="1:36" ht="28.5">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1211,11 +1343,11 @@
     </row>
     <row r="2" spans="1:36">
       <c r="A2" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A3</f>
+        <f>'Capacity factors'!A3</f>
         <v>hard coal</v>
       </c>
       <c r="B2" s="4">
-        <f>'Tabel 1 - Pereira et al'!B3</f>
+        <f>'Capacity factors'!B3</f>
         <v>0.5</v>
       </c>
       <c r="C2" s="4">
@@ -1357,11 +1489,11 @@
     </row>
     <row r="3" spans="1:36">
       <c r="A3" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A4</f>
+        <f>'Capacity factors'!A4</f>
         <v>natural gas nonpeaker</v>
       </c>
       <c r="B3" s="4">
-        <f>'Tabel 1 - Pereira et al'!B4</f>
+        <f>'Capacity factors'!B4</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="C3" s="4">
@@ -1503,11 +1635,11 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A5</f>
+        <f>'Capacity factors'!A5</f>
         <v>nuclear</v>
       </c>
       <c r="B4" s="4">
-        <f>'Tabel 1 - Pereira et al'!B5</f>
+        <f>'Capacity factors'!B5</f>
         <v>0.83</v>
       </c>
       <c r="C4" s="4">
@@ -1649,11 +1781,11 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A6</f>
+        <f>'Capacity factors'!A6</f>
         <v>hydro</v>
       </c>
       <c r="B5" s="4">
-        <f>'Tabel 1 - Pereira et al'!B6</f>
+        <f>'Capacity factors'!B6</f>
         <v>0.495</v>
       </c>
       <c r="C5" s="4">
@@ -1795,11 +1927,11 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A7</f>
+        <f>'Capacity factors'!A7</f>
         <v>onshore wind</v>
       </c>
       <c r="B6" s="4">
-        <f>'Tabel 1 - Pereira et al'!B7</f>
+        <f>'Capacity factors'!B7</f>
         <v>0.39</v>
       </c>
       <c r="C6" s="4">
@@ -1941,11 +2073,11 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A8</f>
+        <f>'Capacity factors'!A8</f>
         <v>solar PV</v>
       </c>
       <c r="B7" s="4">
-        <f>'Tabel 1 - Pereira et al'!B8</f>
+        <f>'Capacity factors'!B8</f>
         <v>0.3</v>
       </c>
       <c r="C7" s="6">
@@ -2087,11 +2219,11 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A9</f>
+        <f>'Capacity factors'!A9</f>
         <v>solar thermal</v>
       </c>
       <c r="B8" s="4">
-        <f>'Tabel 1 - Pereira et al'!B9</f>
+        <f>'Capacity factors'!B9</f>
         <v>0.218</v>
       </c>
       <c r="C8" s="6">
@@ -2233,11 +2365,11 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A10</f>
+        <f>'Capacity factors'!A10</f>
         <v>biomass</v>
       </c>
       <c r="B9" s="4">
-        <f>'Tabel 1 - Pereira et al'!B10</f>
+        <f>'Capacity factors'!B10</f>
         <v>0.245</v>
       </c>
       <c r="C9" s="6">
@@ -2379,11 +2511,11 @@
     </row>
     <row r="10" spans="1:36" s="8" customFormat="1">
       <c r="A10" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A11</f>
+        <f>'Capacity factors'!A11</f>
         <v>geothermal</v>
       </c>
       <c r="B10" s="16">
-        <f>'Tabel 1 - Pereira et al'!B11</f>
+        <f>'Capacity factors'!B11</f>
         <v>0.74</v>
       </c>
       <c r="C10" s="6">
@@ -2525,11 +2657,11 @@
     </row>
     <row r="11" spans="1:36" s="8" customFormat="1">
       <c r="A11" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A12</f>
+        <f>'Capacity factors'!A12</f>
         <v>petroleum</v>
       </c>
       <c r="B11" s="16">
-        <f>'Tabel 1 - Pereira et al'!B12</f>
+        <f>'Capacity factors'!B12</f>
         <v>5.566666666666667E-2</v>
       </c>
       <c r="C11" s="6">
@@ -2671,153 +2803,153 @@
     </row>
     <row r="12" spans="1:36" s="8" customFormat="1">
       <c r="A12" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A13</f>
+        <f>'Capacity factors'!A13</f>
         <v>natural gas peaker</v>
       </c>
       <c r="B12" s="16">
-        <f>'Tabel 1 - Pereira et al'!B13</f>
-        <v>0.55000000000000004</v>
+        <f>'Capacity factors'!B13</f>
+        <v>0.15</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="G12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="N12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="S12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="T12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="U12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="V12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="W12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="X12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="Y12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="Z12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AA12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AB12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AC12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AD12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AE12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AF12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AG12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AH12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AI12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
       <c r="AJ12" s="6">
         <f t="shared" si="2"/>
-        <v>0.55000000000000004</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A14</f>
+        <f>'Capacity factors'!A14</f>
         <v>lignite</v>
       </c>
       <c r="B13" s="4">
@@ -2963,11 +3095,11 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A15</f>
+        <f>'Capacity factors'!A15</f>
         <v>offshore wind</v>
       </c>
       <c r="B14" s="4">
-        <f>'Tabel 1 - Pereira et al'!B15</f>
+        <f>'Capacity factors'!B15</f>
         <v>0.4</v>
       </c>
       <c r="C14" s="6">
@@ -3109,11 +3241,11 @@
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A16</f>
+        <f>'Capacity factors'!A16</f>
         <v>crude oil</v>
       </c>
       <c r="B15" s="4">
-        <f>'Tabel 1 - Pereira et al'!B16</f>
+        <f>'Capacity factors'!B16</f>
         <v>0.2</v>
       </c>
       <c r="C15" s="6">
@@ -3255,11 +3387,11 @@
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A17</f>
+        <f>'Capacity factors'!A17</f>
         <v>heavy or residual fuel oil</v>
       </c>
       <c r="B16" s="4">
-        <f>'Tabel 1 - Pereira et al'!B17</f>
+        <f>'Capacity factors'!B17</f>
         <v>0.54</v>
       </c>
       <c r="C16" s="6">
@@ -3401,11 +3533,11 @@
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="8" t="str">
-        <f>'Tabel 1 - Pereira et al'!A18</f>
+        <f>'Capacity factors'!A18</f>
         <v>municipal solid waste</v>
       </c>
       <c r="B17" s="4">
-        <f>'Tabel 1 - Pereira et al'!B18</f>
+        <f>'Capacity factors'!B18</f>
         <v>0.68</v>
       </c>
       <c r="C17" s="6">
@@ -3557,7 +3689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
@@ -3567,13 +3699,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="4" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.46484375" customWidth="1"/>
+    <col min="2" max="4" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="28.8">
+    <row r="1" spans="1:36" ht="28.5">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -6009,23 +6141,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="4" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.796875" customWidth="1"/>
+    <col min="2" max="4" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="28.8">
+    <row r="1" spans="1:36" ht="28.5">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -6141,7 +6273,7 @@
         <v>hard coal</v>
       </c>
       <c r="B2" s="4">
-        <f>'Tabel 1 - Pereira et al'!C3</f>
+        <f>'Capacity factors'!C3</f>
         <v>0.5</v>
       </c>
       <c r="C2" s="4">
@@ -6287,7 +6419,7 @@
         <v>natural gas nonpeaker</v>
       </c>
       <c r="B3" s="4">
-        <f>'Tabel 1 - Pereira et al'!C4</f>
+        <f>'Capacity factors'!C4</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="C3" s="4">
@@ -6433,7 +6565,7 @@
         <v>nuclear</v>
       </c>
       <c r="B4" s="4">
-        <f>'Tabel 1 - Pereira et al'!C5</f>
+        <f>'Capacity factors'!C5</f>
         <v>0.85</v>
       </c>
       <c r="C4" s="4">
@@ -6579,7 +6711,7 @@
         <v>hydro</v>
       </c>
       <c r="B5" s="4">
-        <f>'Tabel 1 - Pereira et al'!C6</f>
+        <f>'Capacity factors'!C6</f>
         <v>0.56000000000000005</v>
       </c>
       <c r="C5" s="4">
@@ -6725,7 +6857,7 @@
         <v>onshore wind</v>
       </c>
       <c r="B6" s="4">
-        <f>'Tabel 1 - Pereira et al'!C7</f>
+        <f>'Capacity factors'!C7</f>
         <v>0.36499999999999999</v>
       </c>
       <c r="C6" s="4">
@@ -6871,7 +7003,7 @@
         <v>solar PV</v>
       </c>
       <c r="B7" s="4">
-        <f>'Tabel 1 - Pereira et al'!C8</f>
+        <f>'Capacity factors'!C8</f>
         <v>0.3</v>
       </c>
       <c r="C7" s="4">
@@ -7017,7 +7149,7 @@
         <v>solar thermal</v>
       </c>
       <c r="B8" s="4">
-        <f>'Tabel 1 - Pereira et al'!C9</f>
+        <f>'Capacity factors'!C9</f>
         <v>0.67500000000000004</v>
       </c>
       <c r="C8" s="4">
@@ -7163,7 +7295,7 @@
         <v>biomass</v>
       </c>
       <c r="B9" s="4">
-        <f>'Tabel 1 - Pereira et al'!C10</f>
+        <f>'Capacity factors'!C10</f>
         <v>0.47499999999999998</v>
       </c>
       <c r="C9" s="4">
@@ -7309,7 +7441,7 @@
         <v>geothermal</v>
       </c>
       <c r="B10" s="4">
-        <f>'Tabel 1 - Pereira et al'!C11</f>
+        <f>'Capacity factors'!C11</f>
         <v>0.81400000000000006</v>
       </c>
       <c r="C10" s="4">
@@ -7455,7 +7587,7 @@
         <v>petroleum</v>
       </c>
       <c r="B11" s="4">
-        <f>'Tabel 1 - Pereira et al'!C12</f>
+        <f>'Capacity factors'!C12</f>
         <v>6.1233333333333341E-2</v>
       </c>
       <c r="C11" s="4">
@@ -7601,144 +7733,144 @@
         <v>natural gas peaker</v>
       </c>
       <c r="B12" s="4">
-        <f>'Tabel 1 - Pereira et al'!C13</f>
-        <v>0.60500000000000009</v>
+        <f>'Capacity factors'!C13</f>
+        <v>0.15</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="1"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="O12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="S12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="T12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="U12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="V12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="W12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="X12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="Y12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="Z12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AA12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AB12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AC12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AD12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AE12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AF12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AH12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AI12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
       <c r="AJ12" s="4">
         <f t="shared" si="2"/>
-        <v>0.60500000000000009</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:36">
@@ -7893,7 +8025,7 @@
         <v>offshore wind</v>
       </c>
       <c r="B14" s="4">
-        <f>'Tabel 1 - Pereira et al'!C15</f>
+        <f>'Capacity factors'!C15</f>
         <v>0.4</v>
       </c>
       <c r="C14" s="4">
@@ -8039,7 +8171,7 @@
         <v>crude oil</v>
       </c>
       <c r="B15" s="4">
-        <f>'Tabel 1 - Pereira et al'!C16</f>
+        <f>'Capacity factors'!C16</f>
         <v>0.2</v>
       </c>
       <c r="C15" s="4">
@@ -8185,7 +8317,7 @@
         <v>heavy or residual fuel oil</v>
       </c>
       <c r="B16" s="4">
-        <f>'Tabel 1 - Pereira et al'!C17</f>
+        <f>'Capacity factors'!C17</f>
         <v>0.54</v>
       </c>
       <c r="C16" s="4">
@@ -8331,7 +8463,7 @@
         <v>municipal solid waste</v>
       </c>
       <c r="B17" s="4">
-        <f>'Tabel 1 - Pereira et al'!C18</f>
+        <f>'Capacity factors'!C18</f>
         <v>0.748</v>
       </c>
       <c r="C17" s="4">

</xml_diff>